<commit_message>
agregado captador de firma
</commit_message>
<xml_diff>
--- a/public/assets/templates/inspection.xlsx
+++ b/public/assets/templates/inspection.xlsx
@@ -1861,9 +1861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2299680</xdr:colOff>
+      <xdr:colOff>2299320</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>478440</xdr:rowOff>
+      <xdr:rowOff>478080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1877,7 +1877,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="891000" y="399240"/>
-          <a:ext cx="2008800" cy="853200"/>
+          <a:ext cx="2008440" cy="852840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1899,8 +1899,8 @@
   </sheetPr>
   <dimension ref="A1:AL1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE21" activeCellId="0" sqref="AE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30004,8 +30004,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA31" activeCellId="0" sqref="AA31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -55511,7 +55511,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
     <mergeCell ref="D6:L6"/>
     <mergeCell ref="N6:AA6"/>
     <mergeCell ref="D9:G9"/>
@@ -55536,6 +55536,7 @@
     <mergeCell ref="N54:AA54"/>
     <mergeCell ref="D55:L55"/>
     <mergeCell ref="N55:AA55"/>
+    <mergeCell ref="D57:L57"/>
     <mergeCell ref="D58:L58"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>

</xml_diff>

<commit_message>
correcion forma ubicacion beta1.3
</commit_message>
<xml_diff>
--- a/public/assets/templates/inspection.xlsx
+++ b/public/assets/templates/inspection.xlsx
@@ -1751,15 +1751,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -30004,8 +30004,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30013,8 +30013,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="0.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="2.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="4.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="3.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="4.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="4.57"/>
@@ -31803,115 +31803,117 @@
       <c r="AA57" s="192"/>
       <c r="AB57" s="157"/>
     </row>
-    <row r="58" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C58" s="8"/>
-      <c r="D58" s="193"/>
-      <c r="E58" s="193"/>
-      <c r="F58" s="193"/>
-      <c r="G58" s="193"/>
-      <c r="H58" s="193"/>
-      <c r="I58" s="193"/>
-      <c r="J58" s="193"/>
-      <c r="K58" s="193"/>
-      <c r="L58" s="193"/>
-      <c r="M58" s="158"/>
-      <c r="N58" s="194"/>
-      <c r="O58" s="194"/>
-      <c r="P58" s="194"/>
-      <c r="Q58" s="194"/>
-      <c r="R58" s="194"/>
-      <c r="S58" s="194"/>
-      <c r="T58" s="194"/>
-      <c r="U58" s="194"/>
-      <c r="V58" s="194"/>
-      <c r="W58" s="194"/>
-      <c r="X58" s="194"/>
-      <c r="Y58" s="194"/>
-      <c r="Z58" s="194"/>
-      <c r="AA58" s="194"/>
-      <c r="AB58" s="195"/>
-    </row>
-    <row r="59" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="139"/>
-      <c r="D59" s="196"/>
-      <c r="E59" s="196"/>
-      <c r="F59" s="196"/>
-      <c r="G59" s="196"/>
-      <c r="H59" s="196"/>
-      <c r="I59" s="196"/>
-      <c r="J59" s="196"/>
-      <c r="K59" s="196"/>
-      <c r="L59" s="196"/>
-      <c r="M59" s="197"/>
-      <c r="N59" s="196"/>
-      <c r="O59" s="196"/>
-      <c r="P59" s="196"/>
-      <c r="Q59" s="196"/>
-      <c r="R59" s="196"/>
-      <c r="S59" s="196"/>
-      <c r="T59" s="196"/>
-      <c r="U59" s="196"/>
-      <c r="V59" s="196"/>
-      <c r="W59" s="196"/>
-      <c r="X59" s="196"/>
-      <c r="Y59" s="196"/>
-      <c r="Z59" s="196"/>
-      <c r="AA59" s="196"/>
-      <c r="AB59" s="198"/>
-    </row>
-    <row r="60" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="145"/>
-      <c r="E60" s="145"/>
-      <c r="F60" s="145"/>
-      <c r="G60" s="145"/>
-      <c r="H60" s="145"/>
-      <c r="I60" s="145"/>
-      <c r="J60" s="145"/>
-      <c r="K60" s="145"/>
-      <c r="L60" s="145"/>
-      <c r="M60" s="113"/>
-      <c r="N60" s="145"/>
-      <c r="O60" s="145"/>
-      <c r="P60" s="145"/>
-      <c r="Q60" s="145"/>
-      <c r="R60" s="145"/>
-      <c r="S60" s="145"/>
-      <c r="T60" s="145"/>
-      <c r="U60" s="145"/>
-      <c r="V60" s="145"/>
-      <c r="W60" s="145"/>
-      <c r="X60" s="145"/>
-      <c r="Y60" s="145"/>
-      <c r="Z60" s="145"/>
-      <c r="AA60" s="145"/>
-      <c r="AB60" s="113"/>
-    </row>
-    <row r="61" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="145"/>
-      <c r="E61" s="145"/>
-      <c r="F61" s="145"/>
-      <c r="G61" s="145"/>
-      <c r="H61" s="145"/>
-      <c r="I61" s="145"/>
-      <c r="J61" s="145"/>
-      <c r="K61" s="145"/>
-      <c r="L61" s="145"/>
-      <c r="M61" s="113"/>
-      <c r="N61" s="145"/>
-      <c r="O61" s="145"/>
-      <c r="P61" s="145"/>
-      <c r="Q61" s="145"/>
-      <c r="R61" s="145"/>
-      <c r="S61" s="145"/>
-      <c r="T61" s="145"/>
-      <c r="U61" s="145"/>
-      <c r="V61" s="145"/>
-      <c r="W61" s="145"/>
-      <c r="X61" s="145"/>
-      <c r="Y61" s="145"/>
-      <c r="Z61" s="145"/>
-      <c r="AA61" s="145"/>
-      <c r="AB61" s="113"/>
+      <c r="D58" s="190"/>
+      <c r="E58" s="190"/>
+      <c r="F58" s="190"/>
+      <c r="G58" s="190"/>
+      <c r="H58" s="190"/>
+      <c r="I58" s="190"/>
+      <c r="J58" s="190"/>
+      <c r="K58" s="190"/>
+      <c r="L58" s="190"/>
+      <c r="M58" s="190"/>
+      <c r="N58" s="192"/>
+      <c r="O58" s="192"/>
+      <c r="P58" s="192"/>
+      <c r="Q58" s="192"/>
+      <c r="R58" s="192"/>
+      <c r="S58" s="192"/>
+      <c r="T58" s="192"/>
+      <c r="U58" s="192"/>
+      <c r="V58" s="192"/>
+      <c r="W58" s="192"/>
+      <c r="X58" s="192"/>
+      <c r="Y58" s="192"/>
+      <c r="Z58" s="192"/>
+      <c r="AA58" s="192"/>
+      <c r="AB58" s="157"/>
+    </row>
+    <row r="59" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C59" s="8"/>
+      <c r="D59" s="0"/>
+      <c r="E59" s="190"/>
+      <c r="F59" s="190"/>
+      <c r="G59" s="190"/>
+      <c r="H59" s="190"/>
+      <c r="I59" s="190"/>
+      <c r="J59" s="190"/>
+      <c r="K59" s="190"/>
+      <c r="L59" s="190"/>
+      <c r="M59" s="0"/>
+      <c r="N59" s="0"/>
+      <c r="O59" s="0"/>
+      <c r="P59" s="0"/>
+      <c r="Q59" s="0"/>
+      <c r="R59" s="0"/>
+      <c r="S59" s="0"/>
+      <c r="T59" s="0"/>
+      <c r="U59" s="0"/>
+      <c r="V59" s="0"/>
+      <c r="W59" s="0"/>
+      <c r="X59" s="0"/>
+      <c r="Y59" s="0"/>
+      <c r="Z59" s="0"/>
+      <c r="AA59" s="0"/>
+      <c r="AB59" s="193"/>
+    </row>
+    <row r="60" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C60" s="8"/>
+      <c r="D60" s="194"/>
+      <c r="E60" s="194"/>
+      <c r="F60" s="194"/>
+      <c r="G60" s="194"/>
+      <c r="H60" s="194"/>
+      <c r="I60" s="194"/>
+      <c r="J60" s="194"/>
+      <c r="K60" s="194"/>
+      <c r="L60" s="194"/>
+      <c r="M60" s="158"/>
+      <c r="N60" s="195"/>
+      <c r="O60" s="195"/>
+      <c r="P60" s="195"/>
+      <c r="Q60" s="195"/>
+      <c r="R60" s="195"/>
+      <c r="S60" s="195"/>
+      <c r="T60" s="195"/>
+      <c r="U60" s="195"/>
+      <c r="V60" s="195"/>
+      <c r="W60" s="195"/>
+      <c r="X60" s="195"/>
+      <c r="Y60" s="195"/>
+      <c r="Z60" s="195"/>
+      <c r="AA60" s="195"/>
+      <c r="AB60" s="193"/>
+    </row>
+    <row r="61" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C61" s="139"/>
+      <c r="D61" s="196"/>
+      <c r="E61" s="196"/>
+      <c r="F61" s="196"/>
+      <c r="G61" s="196"/>
+      <c r="H61" s="196"/>
+      <c r="I61" s="196"/>
+      <c r="J61" s="196"/>
+      <c r="K61" s="196"/>
+      <c r="L61" s="196"/>
+      <c r="M61" s="197"/>
+      <c r="N61" s="196"/>
+      <c r="O61" s="196"/>
+      <c r="P61" s="196"/>
+      <c r="Q61" s="196"/>
+      <c r="R61" s="196"/>
+      <c r="S61" s="196"/>
+      <c r="T61" s="196"/>
+      <c r="U61" s="196"/>
+      <c r="V61" s="196"/>
+      <c r="W61" s="196"/>
+      <c r="X61" s="196"/>
+      <c r="Y61" s="196"/>
+      <c r="Z61" s="196"/>
+      <c r="AA61" s="196"/>
+      <c r="AB61" s="198"/>
     </row>
     <row r="62" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D62" s="145"/>
@@ -55403,10 +55405,62 @@
       <c r="AA931" s="145"/>
       <c r="AB931" s="113"/>
     </row>
-    <row r="932" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="933" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D932" s="145"/>
+      <c r="E932" s="145"/>
+      <c r="F932" s="145"/>
+      <c r="G932" s="145"/>
+      <c r="H932" s="145"/>
+      <c r="I932" s="145"/>
+      <c r="J932" s="145"/>
+      <c r="K932" s="145"/>
+      <c r="L932" s="145"/>
+      <c r="M932" s="113"/>
+      <c r="N932" s="145"/>
+      <c r="O932" s="145"/>
+      <c r="P932" s="145"/>
+      <c r="Q932" s="145"/>
+      <c r="R932" s="145"/>
+      <c r="S932" s="145"/>
+      <c r="T932" s="145"/>
+      <c r="U932" s="145"/>
+      <c r="V932" s="145"/>
+      <c r="W932" s="145"/>
+      <c r="X932" s="145"/>
+      <c r="Y932" s="145"/>
+      <c r="Z932" s="145"/>
+      <c r="AA932" s="145"/>
+      <c r="AB932" s="113"/>
+    </row>
+    <row r="933" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D933" s="145"/>
+      <c r="E933" s="145"/>
+      <c r="F933" s="145"/>
+      <c r="G933" s="145"/>
+      <c r="H933" s="145"/>
+      <c r="I933" s="145"/>
+      <c r="J933" s="145"/>
+      <c r="K933" s="145"/>
+      <c r="L933" s="145"/>
+      <c r="M933" s="113"/>
+      <c r="N933" s="145"/>
+      <c r="O933" s="145"/>
+      <c r="P933" s="145"/>
+      <c r="Q933" s="145"/>
+      <c r="R933" s="145"/>
+      <c r="S933" s="145"/>
+      <c r="T933" s="145"/>
+      <c r="U933" s="145"/>
+      <c r="V933" s="145"/>
+      <c r="W933" s="145"/>
+      <c r="X933" s="145"/>
+      <c r="Y933" s="145"/>
+      <c r="Z933" s="145"/>
+      <c r="AA933" s="145"/>
+      <c r="AB933" s="113"/>
+    </row>
+    <row r="934" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -55511,7 +55565,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="25">
     <mergeCell ref="D6:L6"/>
     <mergeCell ref="N6:AA6"/>
     <mergeCell ref="D9:G9"/>
@@ -55536,8 +55590,7 @@
     <mergeCell ref="N54:AA54"/>
     <mergeCell ref="D55:L55"/>
     <mergeCell ref="N55:AA55"/>
-    <mergeCell ref="D57:L57"/>
-    <mergeCell ref="D58:L58"/>
+    <mergeCell ref="E57:L59"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.0395833333333333" top="0" bottom="0" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>